<commit_message>
Separé form Equipos. Parece funcionar todo
</commit_message>
<xml_diff>
--- a/Documentos/apk-398.xlsx
+++ b/Documentos/apk-398.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="217">
   <si>
     <t>Mediciones</t>
   </si>
@@ -493,9 +493,6 @@
     <t>PTW</t>
   </si>
   <si>
-    <t>31002/31003 (flexible)</t>
-  </si>
-  <si>
     <t>Victoreen 30-348</t>
   </si>
   <si>
@@ -586,15 +583,6 @@
     <t xml:space="preserve">2505/3, 3B Farmer </t>
   </si>
   <si>
-    <t>NE2571</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Farmer </t>
-  </si>
-  <si>
-    <t>NE2581</t>
-  </si>
-  <si>
     <t xml:space="preserve">2561/2611 Sec. Std </t>
   </si>
   <si>
@@ -685,40 +673,10 @@
     <t>RMI 449</t>
   </si>
   <si>
-    <t>PR06C (Farmer)</t>
-  </si>
-  <si>
-    <t>A2 (Spokas)</t>
-  </si>
-  <si>
-    <t>T2 (Spokas)</t>
-  </si>
-  <si>
-    <t>A12 (Farmer)</t>
-  </si>
-  <si>
-    <t>2571 (Guarded Farmer)</t>
-  </si>
-  <si>
-    <t>2581 (Robust Farmer)</t>
-  </si>
-  <si>
-    <t>30001/30010 (Farmer)</t>
-  </si>
-  <si>
-    <t>30002/30011 (Farmer)</t>
-  </si>
-  <si>
-    <t>30004/30012 (Farmer)</t>
-  </si>
-  <si>
-    <t>30-348</t>
-  </si>
-  <si>
-    <t>30-351</t>
-  </si>
-  <si>
-    <t>30-349</t>
+    <t xml:space="preserve">2571 Farmer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2581 Farmer </t>
   </si>
 </sst>
 </file>
@@ -4670,7 +4628,7 @@
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C80" s="5">
         <v>0.95299999999999996</v>
@@ -5274,7 +5232,7 @@
     </row>
     <row r="92" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -5450,7 +5408,7 @@
     </row>
     <row r="96" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B96" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -5494,7 +5452,7 @@
     </row>
     <row r="97" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -5538,7 +5496,7 @@
     </row>
     <row r="98" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
@@ -5582,7 +5540,7 @@
     </row>
     <row r="99" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
@@ -5635,10 +5593,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S74"/>
+  <dimension ref="A1:S75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:S74"/>
+    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5652,7 +5610,7 @@
         <v>135</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C1" s="5">
         <v>1.004</v>
@@ -5705,7 +5663,7 @@
         <v>135</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" s="5">
         <v>1.004</v>
@@ -5758,7 +5716,7 @@
         <v>135</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" s="5">
         <v>1.0009999999999999</v>
@@ -5811,7 +5769,7 @@
         <v>137</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4" s="5">
         <v>1.0009999999999999</v>
@@ -5864,7 +5822,7 @@
         <v>137</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" s="5">
         <v>1.002</v>
@@ -5917,7 +5875,7 @@
         <v>137</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5">
         <v>1.002</v>
@@ -5970,7 +5928,7 @@
         <v>137</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="5">
         <v>1.0029999999999999</v>
@@ -6023,7 +5981,7 @@
         <v>137</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8" s="5">
         <v>1.0009999999999999</v>
@@ -6073,10 +6031,10 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="C9" s="5">
         <v>1.0049999999999999</v>
@@ -6126,7 +6084,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5">
@@ -6177,10 +6135,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="C11" s="5">
         <v>1.0009999999999999</v>
@@ -6230,10 +6188,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C12" s="5">
         <v>1.0009999999999999</v>
@@ -6283,10 +6241,10 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C13" s="5">
         <v>1.0009999999999999</v>
@@ -6336,10 +6294,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C14" s="5">
         <v>1.0009999999999999</v>
@@ -6389,10 +6347,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C15" s="5">
         <v>1.0009999999999999</v>
@@ -6442,10 +6400,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C16" s="5">
         <v>1.002</v>
@@ -6495,10 +6453,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C17" s="5">
         <v>1.004</v>
@@ -6604,7 +6562,7 @@
         <v>141</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C19" s="5">
         <v>1.0049999999999999</v>
@@ -6710,7 +6668,7 @@
         <v>141</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C21" s="5">
         <v>1.0009999999999999</v>
@@ -6763,7 +6721,7 @@
         <v>141</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C22" s="5">
         <v>1.0049999999999999</v>
@@ -6816,7 +6774,7 @@
         <v>141</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C23" s="5">
         <v>1.0049999999999999</v>
@@ -6869,7 +6827,7 @@
         <v>141</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C24" s="5">
         <v>1.006</v>
@@ -6919,10 +6877,10 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>186</v>
+        <v>141</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="C25" s="5">
         <v>1.0049999999999999</v>
@@ -6972,10 +6930,10 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>188</v>
+        <v>141</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="C26" s="5">
         <v>1.0049999999999999</v>
@@ -7028,7 +6986,7 @@
         <v>141</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C27" s="5">
         <v>1.006</v>
@@ -7081,7 +7039,7 @@
         <v>154</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C28" s="5">
         <v>1.0029999999999999</v>
@@ -7134,7 +7092,7 @@
         <v>154</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C29" s="5">
         <v>1.004</v>
@@ -7187,7 +7145,7 @@
         <v>154</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C30" s="5">
         <v>1.004</v>
@@ -7293,7 +7251,7 @@
         <v>154</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C32" s="5">
         <v>1.004</v>
@@ -7346,7 +7304,7 @@
         <v>154</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C33" s="5">
         <v>1.006</v>
@@ -7399,7 +7357,7 @@
         <v>154</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C34" s="5">
         <v>1.006</v>
@@ -7452,7 +7410,7 @@
         <v>154</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C35" s="5">
         <v>1.002</v>
@@ -7505,7 +7463,7 @@
         <v>154</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C36" s="5">
         <v>1.0029999999999999</v>
@@ -7558,7 +7516,7 @@
         <v>154</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C37" s="5">
         <v>1.0029999999999999</v>
@@ -7608,10 +7566,10 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C38" s="5">
         <v>1.004</v>
@@ -7661,10 +7619,10 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C39" s="5">
         <v>1.006</v>
@@ -7714,10 +7672,10 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C40" s="5">
         <v>1.0049999999999999</v>
@@ -7767,10 +7725,10 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C41" s="5">
         <v>1.0049999999999999</v>
@@ -7820,10 +7778,10 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C42" s="5">
         <v>1.004</v>
@@ -7873,10 +7831,10 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="C43" s="5">
         <v>1.004</v>
@@ -7926,10 +7884,10 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C44" s="5">
         <v>1.0029999999999999</v>
@@ -7979,10 +7937,10 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C45" s="5">
         <v>1.004</v>
@@ -8032,10 +7990,10 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C46" s="5">
         <v>1.0009999999999999</v>
@@ -8085,10 +8043,10 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C47" s="5">
         <v>1.0009999999999999</v>
@@ -8138,10 +8096,10 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C48" s="5">
         <v>1.0009999999999999</v>
@@ -8191,10 +8149,10 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>213</v>
       </c>
       <c r="C49" s="5">
         <v>1.0009999999999999</v>
@@ -8244,10 +8202,10 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C50" s="5">
         <v>1.0009999999999999</v>
@@ -8297,10 +8255,10 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C51" s="5">
         <v>1.0009999999999999</v>
@@ -8350,10 +8308,10 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C52" s="5">
         <v>1.002</v>
@@ -8403,10 +8361,10 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C53" s="5">
         <v>1.004</v>
@@ -8459,7 +8417,7 @@
         <v>134</v>
       </c>
       <c r="B55" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C55">
         <v>0.95299999999999996</v>
@@ -8850,11 +8808,11 @@
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B62" t="s">
-        <v>219</v>
+      <c r="B62" s="5" t="s">
+        <v>163</v>
       </c>
       <c r="I62">
         <v>0.91600000000000004</v>
@@ -8891,11 +8849,11 @@
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B63" t="s">
-        <v>220</v>
+      <c r="B63" s="5" t="s">
+        <v>164</v>
       </c>
       <c r="I63">
         <v>0.91400000000000003</v>
@@ -8932,11 +8890,11 @@
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B64" t="s">
-        <v>221</v>
+      <c r="B64" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="I64">
         <v>0.88200000000000001</v>
@@ -8973,11 +8931,11 @@
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B65" t="s">
-        <v>222</v>
+      <c r="B65" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="I65">
         <v>0.92100000000000004</v>
@@ -9014,11 +8972,11 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B66" t="s">
-        <v>223</v>
+      <c r="B66" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="I66">
         <v>0.91800000000000004</v>
@@ -9055,11 +9013,11 @@
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B67" t="s">
-        <v>224</v>
+      <c r="B67" s="5" t="s">
+        <v>216</v>
       </c>
       <c r="I67">
         <v>0.89900000000000002</v>
@@ -9096,11 +9054,11 @@
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B68" t="s">
-        <v>225</v>
+      <c r="B68" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="I68">
         <v>0.91100000000000003</v>
@@ -9137,11 +9095,11 @@
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B69" t="s">
-        <v>226</v>
+      <c r="B69" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="I69">
         <v>0.91600000000000004</v>
@@ -9178,11 +9136,11 @@
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B70" t="s">
-        <v>227</v>
+      <c r="B70" s="5" t="s">
+        <v>191</v>
       </c>
       <c r="I70">
         <v>0.92</v>
@@ -9219,11 +9177,11 @@
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B71" t="s">
-        <v>155</v>
+      <c r="B71" s="5" t="s">
+        <v>193</v>
       </c>
       <c r="I71">
         <v>0.91200000000000003</v>
@@ -9260,73 +9218,73 @@
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>202</v>
-      </c>
-      <c r="B72" t="s">
-        <v>228</v>
+      <c r="A72" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="I72">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="J72">
         <v>0.91</v>
       </c>
-      <c r="J72">
+      <c r="K72">
         <v>0.90800000000000003</v>
       </c>
-      <c r="K72">
+      <c r="L72">
         <v>0.90600000000000003</v>
       </c>
-      <c r="L72">
+      <c r="M72">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="N72">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="O72">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="P72">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="Q72">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="R72">
+        <v>0.877</v>
+      </c>
+      <c r="S72">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I73">
+        <v>0.91</v>
+      </c>
+      <c r="J73">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="K73">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="L73">
         <v>0.90300000000000002</v>
       </c>
-      <c r="M72">
+      <c r="M73">
         <v>0.90200000000000002</v>
       </c>
-      <c r="N72">
+      <c r="N73">
         <v>0.89800000000000002</v>
       </c>
-      <c r="O72">
+      <c r="O73">
         <v>0.89500000000000002</v>
-      </c>
-      <c r="P72">
-        <v>0.88800000000000001</v>
-      </c>
-      <c r="Q72">
-        <v>0.88</v>
-      </c>
-      <c r="R72">
-        <v>0.872</v>
-      </c>
-      <c r="S72">
-        <v>0.86199999999999999</v>
-      </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>202</v>
-      </c>
-      <c r="B73" t="s">
-        <v>229</v>
-      </c>
-      <c r="I73">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="J73">
-        <v>0.90400000000000003</v>
-      </c>
-      <c r="K73">
-        <v>0.90200000000000002</v>
-      </c>
-      <c r="L73">
-        <v>0.90100000000000002</v>
-      </c>
-      <c r="M73">
-        <v>0.89900000000000002</v>
-      </c>
-      <c r="N73">
-        <v>0.89600000000000002</v>
-      </c>
-      <c r="O73">
-        <v>0.89300000000000002</v>
       </c>
       <c r="P73">
         <v>0.88800000000000001</v>
@@ -9335,54 +9293,96 @@
         <v>0.88</v>
       </c>
       <c r="R73">
-        <v>0.873</v>
+        <v>0.872</v>
       </c>
       <c r="S73">
-        <v>0.86399999999999999</v>
+        <v>0.86199999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B74" t="s">
-        <v>230</v>
-      </c>
       <c r="I74">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="J74">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="K74">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="L74">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="M74">
         <v>0.89900000000000002</v>
       </c>
-      <c r="J74">
-        <v>0.89800000000000002</v>
-      </c>
-      <c r="K74">
-        <v>0.89700000000000002</v>
-      </c>
-      <c r="L74">
+      <c r="N74">
         <v>0.89600000000000002</v>
       </c>
-      <c r="M74">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="N74">
+      <c r="O74">
         <v>0.89300000000000002</v>
-      </c>
-      <c r="O74">
-        <v>0.89100000000000001</v>
       </c>
       <c r="P74">
         <v>0.88800000000000001</v>
       </c>
       <c r="Q74">
+        <v>0.88</v>
+      </c>
+      <c r="R74">
+        <v>0.873</v>
+      </c>
+      <c r="S74">
+        <v>0.86399999999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="I75">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="J75">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="K75">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="L75">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="M75">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="N75">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="O75">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="P75">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="Q75">
         <v>0.88100000000000001</v>
       </c>
-      <c r="R74">
+      <c r="R75">
         <v>0.875</v>
       </c>
-      <c r="S74">
+      <c r="S75">
         <v>0.86599999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Avancé con métodos CaliElectrones
</commit_message>
<xml_diff>
--- a/Documentos/apk-398.xlsx
+++ b/Documentos/apk-398.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="200">
   <si>
     <t>Mediciones</t>
   </si>
@@ -377,57 +377,6 @@
   </si>
   <si>
     <t xml:space="preserve">NE 2515/3 </t>
-  </si>
-  <si>
-    <t>1,0</t>
-  </si>
-  <si>
-    <t>1,4</t>
-  </si>
-  <si>
-    <t>2,0</t>
-  </si>
-  <si>
-    <t>2,5</t>
-  </si>
-  <si>
-    <t>3,0</t>
-  </si>
-  <si>
-    <t>3,5</t>
-  </si>
-  <si>
-    <t>4,0</t>
-  </si>
-  <si>
-    <t>4,5</t>
-  </si>
-  <si>
-    <t>5,0</t>
-  </si>
-  <si>
-    <t>5,5</t>
-  </si>
-  <si>
-    <t>6,0</t>
-  </si>
-  <si>
-    <t>7,0</t>
-  </si>
-  <si>
-    <t>8,0</t>
-  </si>
-  <si>
-    <t>10,0</t>
-  </si>
-  <si>
-    <t>13,0</t>
-  </si>
-  <si>
-    <t>16,0</t>
-  </si>
-  <si>
-    <t>20,0</t>
   </si>
   <si>
     <t>Attix</t>
@@ -1308,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S99"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79:S79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4574,61 +4523,61 @@
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
-      <c r="C79" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="G79" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="H79" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="I79" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="J79" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="K79" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="L79" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="M79" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="N79" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="O79" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="P79" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q79" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="R79" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="S79" s="5" t="s">
-        <v>133</v>
+      <c r="C79" s="5">
+        <v>1</v>
+      </c>
+      <c r="D79" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="E79" s="5">
+        <v>2</v>
+      </c>
+      <c r="F79" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="G79" s="5">
+        <v>3</v>
+      </c>
+      <c r="H79" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="I79" s="5">
+        <v>4</v>
+      </c>
+      <c r="J79" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="K79" s="5">
+        <v>5</v>
+      </c>
+      <c r="L79" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="M79" s="5">
+        <v>6</v>
+      </c>
+      <c r="N79" s="5">
+        <v>7</v>
+      </c>
+      <c r="O79" s="5">
+        <v>8</v>
+      </c>
+      <c r="P79" s="5">
+        <v>10</v>
+      </c>
+      <c r="Q79" s="5">
+        <v>13</v>
+      </c>
+      <c r="R79" s="5">
+        <v>16</v>
+      </c>
+      <c r="S79" s="5">
+        <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="C80" s="5">
         <v>0.95299999999999996</v>
@@ -4684,7 +4633,7 @@
     </row>
     <row r="81" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
@@ -4736,7 +4685,7 @@
     </row>
     <row r="82" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B82" s="5" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="C82" s="5">
         <v>0.95799999999999996</v>
@@ -4792,7 +4741,7 @@
     </row>
     <row r="83" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B83" s="5" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="C83" s="5">
         <v>0.97099999999999997</v>
@@ -4848,7 +4797,7 @@
     </row>
     <row r="84" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="C84" s="5">
         <v>0.95199999999999996</v>
@@ -4904,7 +4853,7 @@
     </row>
     <row r="85" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
@@ -4956,7 +4905,7 @@
     </row>
     <row r="86" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B86" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="C86" s="5">
         <v>0.96499999999999997</v>
@@ -5012,7 +4961,7 @@
     </row>
     <row r="87" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
@@ -5056,7 +5005,7 @@
     </row>
     <row r="88" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B88" s="5" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
@@ -5100,7 +5049,7 @@
     </row>
     <row r="89" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
@@ -5144,7 +5093,7 @@
     </row>
     <row r="90" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
@@ -5188,7 +5137,7 @@
     </row>
     <row r="91" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B91" s="5" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
@@ -5232,7 +5181,7 @@
     </row>
     <row r="92" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -5276,7 +5225,7 @@
     </row>
     <row r="93" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B93" s="5" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
@@ -5320,7 +5269,7 @@
     </row>
     <row r="94" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B94" s="5" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
@@ -5364,7 +5313,7 @@
     </row>
     <row r="95" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B95" s="5" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
@@ -5408,7 +5357,7 @@
     </row>
     <row r="96" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B96" s="5" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -5452,7 +5401,7 @@
     </row>
     <row r="97" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -5496,7 +5445,7 @@
     </row>
     <row r="98" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
@@ -5540,7 +5489,7 @@
     </row>
     <row r="99" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
@@ -5595,8 +5544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5607,10 +5556,10 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="C1" s="5">
         <v>1.004</v>
@@ -5660,10 +5609,10 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C2" s="5">
         <v>1.004</v>
@@ -5713,10 +5662,10 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="C3" s="5">
         <v>1.0009999999999999</v>
@@ -5766,10 +5715,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="C4" s="5">
         <v>1.0009999999999999</v>
@@ -5819,10 +5768,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C5" s="5">
         <v>1.002</v>
@@ -5872,10 +5821,10 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="C6" s="5">
         <v>1.002</v>
@@ -5925,10 +5874,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C7" s="5">
         <v>1.0029999999999999</v>
@@ -5978,10 +5927,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="C8" s="5">
         <v>1.0009999999999999</v>
@@ -6031,10 +5980,10 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="C9" s="5">
         <v>1.0049999999999999</v>
@@ -6084,7 +6033,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5">
@@ -6135,10 +6084,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="C11" s="5">
         <v>1.0009999999999999</v>
@@ -6188,10 +6137,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="C12" s="5">
         <v>1.0009999999999999</v>
@@ -6241,10 +6190,10 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="C13" s="5">
         <v>1.0009999999999999</v>
@@ -6294,10 +6243,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="C14" s="5">
         <v>1.0009999999999999</v>
@@ -6347,10 +6296,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="C15" s="5">
         <v>1.0009999999999999</v>
@@ -6400,10 +6349,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="C16" s="5">
         <v>1.002</v>
@@ -6453,10 +6402,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="C17" s="5">
         <v>1.004</v>
@@ -6506,7 +6455,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B18" s="5">
         <v>2515</v>
@@ -6559,10 +6508,10 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="C19" s="5">
         <v>1.0049999999999999</v>
@@ -6612,7 +6561,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B20" s="5">
         <v>2577</v>
@@ -6665,10 +6614,10 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="C21" s="5">
         <v>1.0009999999999999</v>
@@ -6718,10 +6667,10 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="C22" s="5">
         <v>1.0049999999999999</v>
@@ -6771,10 +6720,10 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C23" s="5">
         <v>1.0049999999999999</v>
@@ -6824,10 +6773,10 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C24" s="5">
         <v>1.006</v>
@@ -6877,10 +6826,10 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C25" s="5">
         <v>1.0049999999999999</v>
@@ -6930,10 +6879,10 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="C26" s="5">
         <v>1.0049999999999999</v>
@@ -6983,10 +6932,10 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="C27" s="5">
         <v>1.006</v>
@@ -7036,10 +6985,10 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="C28" s="5">
         <v>1.0029999999999999</v>
@@ -7089,10 +7038,10 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="C29" s="5">
         <v>1.004</v>
@@ -7142,10 +7091,10 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="C30" s="5">
         <v>1.004</v>
@@ -7195,7 +7144,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B31" s="5">
         <v>23333</v>
@@ -7248,10 +7197,10 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="C32" s="5">
         <v>1.004</v>
@@ -7301,10 +7250,10 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="C33" s="5">
         <v>1.006</v>
@@ -7354,10 +7303,10 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="C34" s="5">
         <v>1.006</v>
@@ -7407,10 +7356,10 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="C35" s="5">
         <v>1.002</v>
@@ -7460,10 +7409,10 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="C36" s="5">
         <v>1.0029999999999999</v>
@@ -7513,10 +7462,10 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="C37" s="5">
         <v>1.0029999999999999</v>
@@ -7566,10 +7515,10 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="C38" s="5">
         <v>1.004</v>
@@ -7619,10 +7568,10 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="C39" s="5">
         <v>1.006</v>
@@ -7672,10 +7621,10 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="C40" s="5">
         <v>1.0049999999999999</v>
@@ -7725,10 +7674,10 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="C41" s="5">
         <v>1.0049999999999999</v>
@@ -7778,10 +7727,10 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="C42" s="5">
         <v>1.004</v>
@@ -7831,10 +7780,10 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="C43" s="5">
         <v>1.004</v>
@@ -7884,10 +7833,10 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="C44" s="5">
         <v>1.0029999999999999</v>
@@ -7937,10 +7886,10 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="C45" s="5">
         <v>1.004</v>
@@ -7990,10 +7939,10 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="C46" s="5">
         <v>1.0009999999999999</v>
@@ -8043,10 +7992,10 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="C47" s="5">
         <v>1.0009999999999999</v>
@@ -8096,10 +8045,10 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="C48" s="5">
         <v>1.0009999999999999</v>
@@ -8149,10 +8098,10 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="C49" s="5">
         <v>1.0009999999999999</v>
@@ -8202,10 +8151,10 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="C50" s="5">
         <v>1.0009999999999999</v>
@@ -8255,10 +8204,10 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="C51" s="5">
         <v>1.0009999999999999</v>
@@ -8308,10 +8257,10 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="C52" s="5">
         <v>1.002</v>
@@ -8361,10 +8310,10 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="C53" s="5">
         <v>1.004</v>
@@ -8414,10 +8363,10 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="B55" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="C55">
         <v>0.95299999999999996</v>
@@ -8473,10 +8422,10 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B56" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="E56">
         <v>0.92100000000000004</v>
@@ -8526,10 +8475,10 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B57" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="C57">
         <v>0.95799999999999996</v>
@@ -8585,7 +8534,7 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="C58">
         <v>0.97099999999999997</v>
@@ -8641,7 +8590,7 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="C59">
         <v>0.95199999999999996</v>
@@ -8697,10 +8646,10 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B60" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="E60">
         <v>0.92500000000000004</v>
@@ -8750,10 +8699,10 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B61" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="C61">
         <v>0.96499999999999997</v>
@@ -8809,10 +8758,10 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="I62">
         <v>0.91600000000000004</v>
@@ -8850,10 +8799,10 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="I63">
         <v>0.91400000000000003</v>
@@ -8891,10 +8840,10 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="I64">
         <v>0.88200000000000001</v>
@@ -8932,10 +8881,10 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="I65">
         <v>0.92100000000000004</v>
@@ -8973,10 +8922,10 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="I66">
         <v>0.91800000000000004</v>
@@ -9014,10 +8963,10 @@
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="I67">
         <v>0.89900000000000002</v>
@@ -9055,10 +9004,10 @@
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="I68">
         <v>0.91100000000000003</v>
@@ -9096,10 +9045,10 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="I69">
         <v>0.91600000000000004</v>
@@ -9137,10 +9086,10 @@
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="I70">
         <v>0.92</v>
@@ -9178,10 +9127,10 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="I71">
         <v>0.91200000000000003</v>
@@ -9219,10 +9168,10 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="I72">
         <v>0.91200000000000003</v>
@@ -9260,10 +9209,10 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="I73">
         <v>0.91</v>
@@ -9301,10 +9250,10 @@
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="I74">
         <v>0.90600000000000003</v>
@@ -9342,10 +9291,10 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="I75">
         <v>0.89900000000000002</v>

</xml_diff>